<commit_message>
exe_moves, count_edges, count_corners works. small bug with D moves
</commit_message>
<xml_diff>
--- a/RotoDNFStats.xlsx
+++ b/RotoDNFStats.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="177"/>
@@ -51,6 +51,12 @@
       <u val="single"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <color rgb="FF6A8759"/>
+      <sz val="9.800000000000001"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -73,7 +79,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -108,6 +114,9 @@
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -455,8 +464,8 @@
   </sheetPr>
   <dimension ref="A1:K990"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.65"/>
@@ -472,8 +481,8 @@
     <col bestFit="1" customWidth="1" max="9" min="9" style="5" width="255.59765625"/>
     <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="255.59765625"/>
     <col bestFit="1" customWidth="1" max="11" min="11" style="1" width="66.86328125"/>
-    <col customWidth="1" max="50" min="12" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="51" style="1" width="9"/>
+    <col customWidth="1" max="51" min="12" style="1" width="9"/>
+    <col customWidth="1" max="16384" min="52" style="1" width="9"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="18.75" r="1">
@@ -529,9 +538,9 @@
       </c>
     </row>
     <row customHeight="1" ht="18.75" r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>U' B' U B' R B2 U F' L' B U2 F' L2 F2 U2 R2 B2 D2 F R2</t>
+      <c r="A2" s="13" t="inlineStr">
+        <is>
+          <t>B2 F2 U2 F2 D R2 U' L2 D L2 F2 B' R' U B2 D R D' L B U'</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -549,9 +558,9 @@
       <c r="K2" s="11" t="n"/>
     </row>
     <row customHeight="1" ht="18.75" r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>U' B' U B' R B2 U F' L' B U2 F' L2 F2 U2 R2 B2 D2 F R2</t>
+      <c r="A3" s="13" t="inlineStr">
+        <is>
+          <t>B2 F2 U2 F2 D R2 U' L2 D L2 F2 B' R' U B2 D R D' L B U'</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
@@ -567,9 +576,9 @@
       <c r="J3" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="18.75" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>U' B' U B' R B2 U F' L' B U2 F' L2 F2 U2 R2 B2 D2 F R2</t>
+      <c r="A4" s="13" t="inlineStr">
+        <is>
+          <t>B2 F2 U2 F2 D R2 U' L2 D L2 F2 B' R' U B2 D R D' L B U'</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
@@ -577,17 +586,43 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>10.82</v>
+      </c>
+      <c r="D4" t="n">
+        <v>33.96</v>
+      </c>
+      <c r="E4" t="n">
+        <v>44.78</v>
+      </c>
+      <c r="F4" t="n">
+        <v>37</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="H4" s="10" t="inlineStr">
         <is>
           <t>solve4</t>
         </is>
       </c>
-      <c r="J4" s="8" t="n"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> D D U' R' U' D B B U D' R' U D' D' U' D B' U D' R U' R' U' D B U U D' U' R' L F R' L D' D' R L' F R L' U D' F U' D R' U' R U D' F' U D R' L F R F B' D' D' F' B R F' L' R R U' R' U R' L F' R F L' R2 L2 D R L' F' F' R' L D R' L R' L R U U R D R' U U R D' R' R'</t>
+        </is>
+      </c>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=B2_F2_U2_F2_D_R2_U-_L2_D_L2_F2_B-_R-_U_B2_D_R_D-_L_B_U-%0A&amp;alg=_D_D_U-_R-_U-_D_B_B_U_D-_R-_U_D-_D-_U-_D_B-_U_D-_R_U-_R-_U-_D_B_U_U_D-_U-_R-_L_F_R-_L_D-_D-_R_L-_F_R_L-_U_D-_F_U-_D_R-_U-_R_U_D-_F-_U_D_R-_L_F_R_F_B-_D-_D-_F-_B_R_F-_L-_R_R_U-_R-_U_R-_L_F-_R_F_L-_R2_L2_D_R_L-_F-_F-_R-_L_D_R-_L_R-_L_%2F%2Fmistake_from_here%0AR_U_U_R_D_R-_U_U_R_D-_R-_R-_%0A</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>U' B' U B' R B2 U F' L' B U2 F' L2 F2 U2 R2 B2 D2 F R2</t>
+      <c r="A5" s="13" t="inlineStr">
+        <is>
+          <t>B2 F2 U2 F2 D R2 U' L2 D L2 F2 B' R' U B2 D R D' L B U'</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
@@ -603,9 +638,9 @@
       <c r="J5" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="18.75" r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>U' B' U B' R B2 U F' L' B U2 F' L2 F2 U2 R2 B2 D2 F R2</t>
+      <c r="A6" s="13" t="inlineStr">
+        <is>
+          <t>B2 F2 U2 F2 D R2 U' L2 D L2 F2 B' R' U B2 D R D' L B U'</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
@@ -622,9 +657,9 @@
       <c r="J6" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="18.75" r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>U' B' U B' R B2 U F' L' B U2 F' L2 F2 U2 R2 B2 D2 F R2</t>
+      <c r="A7" s="13" t="inlineStr">
+        <is>
+          <t>B2 F2 U2 F2 D R2 U' L2 D L2 F2 B' R' U B2 D R D' L B U'</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
@@ -632,17 +667,43 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>6.06</v>
+      </c>
+      <c r="D7" t="n">
+        <v>48.4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>54.46</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="H7" s="10" t="inlineStr">
         <is>
           <t>solve7</t>
         </is>
       </c>
-      <c r="J7" s="8" t="n"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> D U' D R' U' D B B U D' R' D' U D' U' D B' U D' R U' R' U' D B U D' U U' R' L F R' L D' D' R L' F R L' U D' F U' D R' U' R U D' F' U D R' L F R F B' D' D' F' B R F' L' R L' U L U' R' L F L' F' R R U U R D R' U2 R D' R' R' R U R D' R' U' R D R' R' R' U D' R' D R U' R' D' R D R D' L' D L D' L' D R' D' L D L' D' L D R</t>
+        </is>
+      </c>
+      <c r="J7" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=B2_F2_U2_F2_D_R2_U-_L2_D_L2_F2_B-_R-_U_B2_D_R_D-_L_B_U-%0A&amp;alg=_D_U-_D_R-_U-_D_B_B_U_D-_R-_D-_U_D-_U-_D_B-_U_D-_R_U-_R-_U-_D_B_U_D-_U_U-_R-_L_F_R-_L_D-_D-_R_L-_F_R_L-_U_D-_F_U-_D_R-_U-_R_U_D-_F-_U_D_R-_L_F_R_F_B-_D-_D-_F-_B_R_F-_L-_R_L-_U_L_U-_R-_L_F_L-_F-_R_R_U_U_R_D_R-_U2_R_D-_R-_R-_R_U_R_D-_R-_U-_R_D_R-_R-_R-_U_D-_R-_D_R_U-_R-_D-_R_D_R_D-_L-_D_L_D-_L-_D_R-_D-_L_D_L-_D-_L_D_R%0A</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>U' B' U B' R B2 U F' L' B U2 F' L2 F2 U2 R2 B2 D2 F R2</t>
+      <c r="A8" s="13" t="inlineStr">
+        <is>
+          <t>B2 F2 U2 F2 D R2 U' L2 D L2 F2 B' R' U B2 D R D' L B U'</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -650,18 +711,43 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D8" t="n">
+        <v>25.62</v>
+      </c>
+      <c r="E8" t="n">
+        <v>31.79</v>
+      </c>
+      <c r="F8" t="n">
+        <v>24</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="H8" s="10" t="inlineStr">
         <is>
           <t>solve8</t>
         </is>
       </c>
-      <c r="I8" s="12" t="n"/>
-      <c r="J8" s="8" t="n"/>
+      <c r="I8" s="12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> D D U' R' U' D B2 U D' R' U D' D' U' D B' U D' R U' R' U' D B U2 D' U' R' L F R' L D2 R L' F R L' U D' F U' D R' U' R U D' F' U D R' L F R F B' D' D' F' B R F' L' R L' U L U' R' L F L' F' R R U2 R D R' U U R D' R' R' R U R D' R' U' R D R' R' R R R D D U' R'</t>
+        </is>
+      </c>
+      <c r="J8" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=B2_F2_U2_F2_D_R2_U-_L2_D_L2_F2_B-_R-_U_B2_D_R_D-_L_B_U-%0A&amp;alg=_D_D_U-_R-_U-_D_B2_U_D-_R-_U_D-_D-_U-_D_B-_U_D-_R_U-_R-_U-_D_B_U2_D-_U-_R-_L_F_R-_L_D2_R_L-_F_R_L-_U_D-_F_U-_D_R-_U-_R_U_D-_F-_U_D_R-_L_F_R_F_B-_D-_D-_F-_B_R_F-_L-_R_L-_U_L_U-_R-_L_F_L-_F-_R_R_U2_R_D_R-_U_U_R_D-_R-_R-_R_U_R_D-_R-_U-_R_D_R-_R-_%2F%2Fmistake_from_here%0AR_R_R_D_D_U-_R-_%0A</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>U' B' U B' R B2 U F' L' B U2 F' L2 F2 U2 R2 B2 D2 F R2</t>
+      <c r="A9" s="13" t="inlineStr">
+        <is>
+          <t>B2 F2 U2 F2 D R2 U' L2 D L2 F2 B' R' U B2 D R D' L B U'</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
@@ -1979,7 +2065,7 @@
       </c>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H63" s="10" t="inlineStr">
@@ -1997,7 +2083,7 @@
       </c>
       <c r="B64" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H64" s="10" t="inlineStr">
@@ -2015,6 +2101,23 @@
       </c>
       <c r="B65" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>12.24</v>
+      </c>
+      <c r="D65" t="n">
+        <v>53.78</v>
+      </c>
+      <c r="E65" t="n">
+        <v>66.03</v>
+      </c>
+      <c r="F65" t="n">
+        <v>58</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2023,7 +2126,16 @@
           <t>solve65</t>
         </is>
       </c>
-      <c r="J65" s="8" t="n"/>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> R2 F U D' F' F' U' D R R F' R' R' R R2 F U D' F' F' U' D R R F' R' R' D F' U D' L L U' D F' D' D F' U D' L L U' D F' D' R U R' U' R' L F R F' L' B R' L L F' L' F L' R U' L U L' B' R2 U' R R</t>
+        </is>
+      </c>
+      <c r="J65" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=B-_L_F2_U2_F2_U-_R2_U-_F2_L2_U_R2_U-_F-_L2_U-_B_L_D_U_B_%0A&amp;alg=_R2_F_U_D-_F-_F-_U-_D_R_R_F-_R-_R-_R_R2_F_U_D-_F-_F-_U-_D_R_R_F-_R-_R-_D_F-_U_D-_L_L_U-_D_F-_D-_D_F-_U_D-_L_L_U-_D_F-_D-_R_U_R-_U-_R-_L_F_R_F-_L-_B_R-_L_L_F-_L-_F_L-_R_U-_L_U_L-_B-_%2F%2Fmistake_from_here%0AR2_U-_R_R_%0A</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="66">
       <c r="A66" s="3" t="inlineStr">
@@ -2033,7 +2145,7 @@
       </c>
       <c r="B66" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H66" s="10" t="inlineStr">

</xml_diff>

<commit_message>
trainer works, WPS small bugs
</commit_message>
<xml_diff>
--- a/RotoDNFStats.xlsx
+++ b/RotoDNFStats.xlsx
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B70" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H70" s="10" t="inlineStr">
@@ -2235,7 +2235,7 @@
       </c>
       <c r="B71" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H71" s="10" t="inlineStr">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B72" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H72" s="10" t="inlineStr">
@@ -2271,7 +2271,24 @@
       </c>
       <c r="B73" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="D73" t="n">
+        <v>45.02</v>
+      </c>
+      <c r="E73" t="n">
+        <v>65.31999999999999</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>yes</t>
         </is>
       </c>
       <c r="H73" s="10" t="inlineStr">
@@ -2279,7 +2296,11 @@
           <t>solve73</t>
         </is>
       </c>
-      <c r="J73" s="8" t="n"/>
+      <c r="J73" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=R_F-_D-_B2_R_U-_B-_L-_B2_U2_R2_D_F2_R2_U_R2_B2_U-_D-_F2_L-%0A&amp;alg=%0A</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="74">
       <c r="A74" s="3" t="inlineStr">
@@ -2289,7 +2310,7 @@
       </c>
       <c r="B74" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H74" s="10" t="inlineStr">
@@ -2307,7 +2328,7 @@
       </c>
       <c r="B75" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H75" s="10" t="inlineStr">
@@ -2325,7 +2346,7 @@
       </c>
       <c r="B76" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H76" s="10" t="inlineStr">
@@ -2343,7 +2364,7 @@
       </c>
       <c r="B77" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H77" s="10" t="inlineStr">
@@ -2361,7 +2382,7 @@
       </c>
       <c r="B78" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H78" s="10" t="inlineStr">
@@ -2379,7 +2400,7 @@
       </c>
       <c r="B79" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H79" s="10" t="inlineStr">
@@ -2397,6 +2418,23 @@
       </c>
       <c r="B80" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="D80" t="n">
+        <v>64.08</v>
+      </c>
+      <c r="E80" t="n">
+        <v>70.33</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2405,7 +2443,11 @@
           <t>solve80</t>
         </is>
       </c>
-      <c r="J80" s="8" t="n"/>
+      <c r="J80" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=L-_U-_F2_D_L2_U2_L2_R2_B2_L2_R2_U_R-_F-_D_L_U-_R_B_L-_%0A&amp;alg=%0A</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="81">
       <c r="A81" s="3" t="inlineStr">
@@ -2415,6 +2457,23 @@
       </c>
       <c r="B81" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="D81" t="n">
+        <v>45.94</v>
+      </c>
+      <c r="E81" t="n">
+        <v>51.74</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2423,7 +2482,16 @@
           <t>solve81</t>
         </is>
       </c>
-      <c r="J81" s="8" t="n"/>
+      <c r="J81" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=D2_L2_U2_B2_U-_R2_F2_U_B2_U_F2_L-_D2_B-_F_D_L_D-_F2_D-_U2_%0A&amp;alg=%0A</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>trace_error</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="82">
       <c r="A82" s="3" t="inlineStr">
@@ -2433,6 +2501,23 @@
       </c>
       <c r="B82" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>8.359999999999999</v>
+      </c>
+      <c r="D82" t="n">
+        <v>127.95</v>
+      </c>
+      <c r="E82" t="n">
+        <v>136.3</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2441,7 +2526,16 @@
           <t>solve82</t>
         </is>
       </c>
-      <c r="J82" s="8" t="n"/>
+      <c r="J82" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=F2_D-_L2_F-_B-_R-_D2_F2_L_D_L2_D-_B2_L2_U-_L2_D2_R2_L2_F2_D-_%0A&amp;alg=%0A</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>trace_error</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="83">
       <c r="A83" s="3" t="inlineStr">
@@ -2451,6 +2545,23 @@
       </c>
       <c r="B83" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D83" t="n">
+        <v>31.91</v>
+      </c>
+      <c r="E83" t="n">
+        <v>36.6</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2459,7 +2570,16 @@
           <t>solve83</t>
         </is>
       </c>
-      <c r="J83" s="8" t="n"/>
+      <c r="J83" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=D2_F_L2_B-_U2_B2_R2_D2_L2_B_U2_F2_R_B_D_L2_R-_U-_F_R_F2_%0A&amp;alg=%0A</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>trace_error</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="84">
       <c r="A84" s="3" t="inlineStr">
@@ -2469,6 +2589,23 @@
       </c>
       <c r="B84" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>10.19</v>
+      </c>
+      <c r="D84" t="n">
+        <v>131.42</v>
+      </c>
+      <c r="E84" t="n">
+        <v>141.61</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2477,7 +2614,16 @@
           <t>solve84</t>
         </is>
       </c>
-      <c r="J84" s="8" t="n"/>
+      <c r="J84" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=B2_L_F2_B_U_B-_R-_L_B2_D-_B2_D-_B2_U_F2_D2_R2_B2_U_R-%0A&amp;alg=%0A</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>trace_error</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="85">
       <c r="A85" s="3" t="inlineStr">
@@ -2487,6 +2633,23 @@
       </c>
       <c r="B85" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="D85" t="n">
+        <v>65.72</v>
+      </c>
+      <c r="E85" t="n">
+        <v>70.33</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2495,7 +2658,16 @@
           <t>solve85</t>
         </is>
       </c>
-      <c r="J85" s="8" t="n"/>
+      <c r="J85" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=D2_F2_D2_B2_U2_R2_F_U2_L2_F_D2_L_B-_L2_B_F2_D_B_R_D2%0A&amp;alg=%0A</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>trace_error</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="86">
       <c r="A86" s="3" t="inlineStr">
@@ -2505,7 +2677,7 @@
       </c>
       <c r="B86" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H86" s="10" t="inlineStr">
@@ -2523,7 +2695,7 @@
       </c>
       <c r="B87" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H87" s="10" t="inlineStr">
@@ -2541,7 +2713,7 @@
       </c>
       <c r="B88" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H88" s="10" t="inlineStr">
@@ -2559,7 +2731,7 @@
       </c>
       <c r="B89" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H89" s="10" t="inlineStr">
@@ -2577,7 +2749,7 @@
       </c>
       <c r="B90" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H90" s="10" t="inlineStr">
@@ -2595,7 +2767,7 @@
       </c>
       <c r="B91" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H91" s="10" t="inlineStr">
@@ -2613,7 +2785,7 @@
       </c>
       <c r="B92" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H92" s="10" t="inlineStr">
@@ -2631,7 +2803,7 @@
       </c>
       <c r="B93" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H93" s="10" t="inlineStr">
@@ -2649,7 +2821,7 @@
       </c>
       <c r="B94" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H94" s="10" t="inlineStr">
@@ -2667,7 +2839,7 @@
       </c>
       <c r="B95" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H95" s="10" t="inlineStr">
@@ -2685,7 +2857,7 @@
       </c>
       <c r="B96" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H96" s="10" t="inlineStr">
@@ -2703,7 +2875,7 @@
       </c>
       <c r="B97" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H97" s="10" t="inlineStr">
@@ -2721,7 +2893,7 @@
       </c>
       <c r="B98" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H98" s="10" t="inlineStr">
@@ -2739,7 +2911,7 @@
       </c>
       <c r="B99" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H99" s="10" t="inlineStr">
@@ -2757,7 +2929,24 @@
       </c>
       <c r="B100" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>40.6</v>
+      </c>
+      <c r="D100" t="n">
+        <v>54.83</v>
+      </c>
+      <c r="E100" t="n">
+        <v>95.43000000000001</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>yes</t>
         </is>
       </c>
       <c r="H100" s="10" t="inlineStr">
@@ -2765,7 +2954,16 @@
           <t>solve100</t>
         </is>
       </c>
-      <c r="J100" s="8" t="n"/>
+      <c r="J100" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=L2_F2_L2_U-_L2_D-_B2_U_F2_U-_B2_U-_F_R-_D_F_R2_F2_R_U-_L2%0A&amp;alg=%0A</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>exe_error</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="101">
       <c r="A101" s="3" t="inlineStr">
@@ -2775,6 +2973,23 @@
       </c>
       <c r="B101" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>17.36</v>
+      </c>
+      <c r="D101" t="n">
+        <v>71.12</v>
+      </c>
+      <c r="E101" t="n">
+        <v>88.48</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2783,7 +2998,16 @@
           <t>solve101</t>
         </is>
       </c>
-      <c r="J101" s="8" t="n"/>
+      <c r="J101" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=L-_F2_L2_U-_R2_B2_D_L2_U-_L2_U-_R-_D2_U2_R-_D2_L2_U-_F-_%0A&amp;alg=%0A</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>trace_error</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="102">
       <c r="A102" s="3" t="inlineStr">
@@ -2793,7 +3017,7 @@
       </c>
       <c r="B102" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H102" s="10" t="inlineStr">
@@ -2811,6 +3035,23 @@
       </c>
       <c r="B103" s="1" t="inlineStr">
         <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>15.97</v>
+      </c>
+      <c r="D103" t="n">
+        <v>49.84</v>
+      </c>
+      <c r="E103" t="n">
+        <v>65.81</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
@@ -2819,7 +3060,16 @@
           <t>solve103</t>
         </is>
       </c>
-      <c r="J103" s="8" t="n"/>
+      <c r="J103" s="8" t="inlineStr">
+        <is>
+          <t>https://alg.cubing.net/?setup=F2_R-_B2_L2_D2_R2_U-_F2_R2_U_L2_U-_F2_U_F-_D_B-_L2_D-_L_F-_%0A&amp;alg=%0A</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>exe_error</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18.75" r="104">
       <c r="A104" s="3" t="inlineStr">
@@ -2829,7 +3079,7 @@
       </c>
       <c r="B104" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H104" s="10" t="inlineStr">
@@ -2847,7 +3097,7 @@
       </c>
       <c r="B105" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H105" s="10" t="inlineStr">
@@ -2865,7 +3115,7 @@
       </c>
       <c r="B106" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H106" s="10" t="inlineStr">
@@ -2883,7 +3133,7 @@
       </c>
       <c r="B107" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H107" s="10" t="inlineStr">
@@ -2901,7 +3151,7 @@
       </c>
       <c r="B108" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H108" s="10" t="inlineStr">
@@ -2919,7 +3169,7 @@
       </c>
       <c r="B109" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H109" s="10" t="inlineStr">
@@ -2937,7 +3187,7 @@
       </c>
       <c r="B110" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H110" s="10" t="inlineStr">
@@ -2955,7 +3205,7 @@
       </c>
       <c r="B111" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H111" s="10" t="inlineStr">
@@ -2973,7 +3223,7 @@
       </c>
       <c r="B112" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H112" s="10" t="inlineStr">
@@ -2991,7 +3241,7 @@
       </c>
       <c r="B113" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H113" s="10" t="inlineStr">
@@ -3009,7 +3259,7 @@
       </c>
       <c r="B114" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H114" s="10" t="inlineStr">
@@ -3027,7 +3277,7 @@
       </c>
       <c r="B115" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H115" s="10" t="inlineStr">
@@ -3045,7 +3295,7 @@
       </c>
       <c r="B116" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H116" s="10" t="inlineStr">
@@ -3063,7 +3313,7 @@
       </c>
       <c r="B117" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H117" s="10" t="inlineStr">
@@ -3081,7 +3331,7 @@
       </c>
       <c r="B118" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H118" s="10" t="inlineStr">
@@ -3099,7 +3349,7 @@
       </c>
       <c r="B119" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H119" s="10" t="inlineStr">
@@ -3117,7 +3367,7 @@
       </c>
       <c r="B120" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H120" s="10" t="inlineStr">
@@ -3135,7 +3385,7 @@
       </c>
       <c r="B121" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H121" s="10" t="inlineStr">
@@ -3153,7 +3403,7 @@
       </c>
       <c r="B122" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H122" s="10" t="inlineStr">
@@ -3171,7 +3421,7 @@
       </c>
       <c r="B123" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H123" s="10" t="inlineStr">
@@ -3189,7 +3439,7 @@
       </c>
       <c r="B124" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H124" s="10" t="inlineStr">
@@ -3207,7 +3457,7 @@
       </c>
       <c r="B125" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H125" s="10" t="inlineStr">
@@ -3225,7 +3475,7 @@
       </c>
       <c r="B126" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H126" s="10" t="inlineStr">
@@ -3243,7 +3493,7 @@
       </c>
       <c r="B127" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H127" s="10" t="inlineStr">
@@ -3261,7 +3511,7 @@
       </c>
       <c r="B128" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H128" s="10" t="inlineStr">
@@ -3279,7 +3529,7 @@
       </c>
       <c r="B129" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H129" s="10" t="inlineStr">
@@ -3297,7 +3547,7 @@
       </c>
       <c r="B130" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H130" s="10" t="inlineStr">
@@ -3315,7 +3565,7 @@
       </c>
       <c r="B131" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H131" s="10" t="inlineStr">
@@ -3333,7 +3583,7 @@
       </c>
       <c r="B132" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H132" s="10" t="inlineStr">
@@ -3351,7 +3601,7 @@
       </c>
       <c r="B133" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H133" s="10" t="inlineStr">
@@ -3369,7 +3619,7 @@
       </c>
       <c r="B134" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H134" s="10" t="inlineStr">
@@ -3387,7 +3637,7 @@
       </c>
       <c r="B135" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H135" s="10" t="inlineStr">
@@ -3405,7 +3655,7 @@
       </c>
       <c r="B136" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H136" s="10" t="inlineStr">
@@ -3423,7 +3673,7 @@
       </c>
       <c r="B137" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H137" s="10" t="inlineStr">
@@ -3441,7 +3691,7 @@
       </c>
       <c r="B138" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H138" s="10" t="inlineStr">
@@ -3459,7 +3709,7 @@
       </c>
       <c r="B139" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H139" s="10" t="inlineStr">
@@ -3477,7 +3727,7 @@
       </c>
       <c r="B140" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H140" s="10" t="inlineStr">
@@ -3495,7 +3745,7 @@
       </c>
       <c r="B141" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H141" s="10" t="inlineStr">
@@ -3513,7 +3763,7 @@
       </c>
       <c r="B142" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H142" s="10" t="inlineStr">
@@ -3531,7 +3781,7 @@
       </c>
       <c r="B143" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H143" s="10" t="inlineStr">
@@ -3549,7 +3799,7 @@
       </c>
       <c r="B144" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H144" s="10" t="inlineStr">
@@ -3567,7 +3817,7 @@
       </c>
       <c r="B145" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H145" s="10" t="inlineStr">
@@ -3585,7 +3835,7 @@
       </c>
       <c r="B146" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H146" s="10" t="inlineStr">
@@ -3603,7 +3853,7 @@
       </c>
       <c r="B147" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H147" s="10" t="inlineStr">
@@ -3621,7 +3871,7 @@
       </c>
       <c r="B148" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H148" s="10" t="inlineStr">
@@ -3639,7 +3889,7 @@
       </c>
       <c r="B149" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H149" s="10" t="inlineStr">
@@ -3657,7 +3907,7 @@
       </c>
       <c r="B150" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H150" s="10" t="inlineStr">
@@ -3675,7 +3925,7 @@
       </c>
       <c r="B151" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H151" s="10" t="inlineStr">
@@ -3693,7 +3943,7 @@
       </c>
       <c r="B152" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H152" s="10" t="inlineStr">
@@ -3711,7 +3961,7 @@
       </c>
       <c r="B153" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H153" s="10" t="inlineStr">
@@ -3729,7 +3979,7 @@
       </c>
       <c r="B154" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H154" s="10" t="inlineStr">
@@ -3747,7 +3997,7 @@
       </c>
       <c r="B155" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H155" s="10" t="inlineStr">
@@ -3765,7 +4015,7 @@
       </c>
       <c r="B156" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H156" s="10" t="inlineStr">
@@ -3783,7 +4033,7 @@
       </c>
       <c r="B157" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H157" s="10" t="inlineStr">
@@ -3801,7 +4051,7 @@
       </c>
       <c r="B158" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H158" s="10" t="inlineStr">
@@ -3819,7 +4069,7 @@
       </c>
       <c r="B159" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H159" s="10" t="inlineStr">
@@ -3837,7 +4087,7 @@
       </c>
       <c r="B160" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H160" s="10" t="inlineStr">
@@ -3855,7 +4105,7 @@
       </c>
       <c r="B161" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H161" s="10" t="inlineStr">
@@ -3873,7 +4123,7 @@
       </c>
       <c r="B162" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H162" s="10" t="inlineStr">
@@ -3891,7 +4141,7 @@
       </c>
       <c r="B163" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H163" s="10" t="inlineStr">
@@ -3909,7 +4159,7 @@
       </c>
       <c r="B164" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H164" s="10" t="inlineStr">
@@ -3927,7 +4177,7 @@
       </c>
       <c r="B165" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H165" s="10" t="inlineStr">
@@ -3945,7 +4195,7 @@
       </c>
       <c r="B166" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H166" s="10" t="inlineStr">
@@ -3963,7 +4213,7 @@
       </c>
       <c r="B167" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H167" s="10" t="inlineStr">
@@ -3981,7 +4231,7 @@
       </c>
       <c r="B168" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H168" s="10" t="inlineStr">
@@ -3999,7 +4249,7 @@
       </c>
       <c r="B169" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H169" s="10" t="inlineStr">
@@ -4017,7 +4267,7 @@
       </c>
       <c r="B170" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H170" s="10" t="inlineStr">
@@ -4035,7 +4285,7 @@
       </c>
       <c r="B171" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H171" s="10" t="inlineStr">
@@ -4053,7 +4303,7 @@
       </c>
       <c r="B172" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H172" s="10" t="inlineStr">
@@ -4071,7 +4321,7 @@
       </c>
       <c r="B173" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H173" s="10" t="inlineStr">
@@ -4089,7 +4339,7 @@
       </c>
       <c r="B174" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H174" s="10" t="inlineStr">
@@ -4107,7 +4357,7 @@
       </c>
       <c r="B175" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H175" s="10" t="inlineStr">
@@ -4125,7 +4375,7 @@
       </c>
       <c r="B176" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H176" s="10" t="inlineStr">
@@ -4143,7 +4393,7 @@
       </c>
       <c r="B177" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H177" s="10" t="inlineStr">
@@ -4161,7 +4411,7 @@
       </c>
       <c r="B178" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H178" s="10" t="inlineStr">
@@ -4179,7 +4429,7 @@
       </c>
       <c r="B179" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H179" s="10" t="inlineStr">
@@ -4197,7 +4447,7 @@
       </c>
       <c r="B180" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H180" s="10" t="inlineStr">
@@ -4215,7 +4465,7 @@
       </c>
       <c r="B181" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H181" s="10" t="inlineStr">
@@ -4233,7 +4483,7 @@
       </c>
       <c r="B182" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H182" s="10" t="inlineStr">
@@ -4251,7 +4501,7 @@
       </c>
       <c r="B183" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H183" s="10" t="inlineStr">
@@ -4269,7 +4519,7 @@
       </c>
       <c r="B184" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H184" s="10" t="inlineStr">
@@ -4287,7 +4537,7 @@
       </c>
       <c r="B185" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H185" s="10" t="inlineStr">
@@ -4305,7 +4555,7 @@
       </c>
       <c r="B186" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H186" s="10" t="inlineStr">
@@ -4323,7 +4573,7 @@
       </c>
       <c r="B187" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H187" s="10" t="inlineStr">
@@ -4341,7 +4591,7 @@
       </c>
       <c r="B188" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H188" s="10" t="inlineStr">
@@ -4359,7 +4609,7 @@
       </c>
       <c r="B189" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H189" s="10" t="inlineStr">
@@ -4377,7 +4627,7 @@
       </c>
       <c r="B190" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H190" s="10" t="inlineStr">
@@ -4395,7 +4645,7 @@
       </c>
       <c r="B191" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H191" s="10" t="inlineStr">
@@ -4413,7 +4663,7 @@
       </c>
       <c r="B192" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H192" s="10" t="inlineStr">
@@ -4431,7 +4681,7 @@
       </c>
       <c r="B193" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H193" s="10" t="inlineStr">
@@ -4449,7 +4699,7 @@
       </c>
       <c r="B194" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H194" s="10" t="inlineStr">
@@ -4467,7 +4717,7 @@
       </c>
       <c r="B195" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H195" s="10" t="inlineStr">
@@ -4485,7 +4735,7 @@
       </c>
       <c r="B196" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H196" s="10" t="inlineStr">
@@ -4503,7 +4753,7 @@
       </c>
       <c r="B197" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H197" s="10" t="inlineStr">
@@ -4521,7 +4771,7 @@
       </c>
       <c r="B198" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H198" s="10" t="inlineStr">
@@ -4539,7 +4789,7 @@
       </c>
       <c r="B199" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H199" s="10" t="inlineStr">
@@ -4557,7 +4807,7 @@
       </c>
       <c r="B200" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H200" s="10" t="inlineStr">

</xml_diff>

<commit_message>
fixed recording issues, saving results
</commit_message>
<xml_diff>
--- a/RotoDNFStats.xlsx
+++ b/RotoDNFStats.xlsx
@@ -4825,7 +4825,7 @@
       </c>
       <c r="B201" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H201" s="10" t="inlineStr">
@@ -4843,7 +4843,7 @@
       </c>
       <c r="B202" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H202" s="10" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="B203" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H203" s="10" t="inlineStr">
@@ -4879,7 +4879,7 @@
       </c>
       <c r="B204" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H204" s="10" t="inlineStr">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="B205" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H205" s="10" t="inlineStr">
@@ -4915,7 +4915,7 @@
       </c>
       <c r="B206" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H206" s="10" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="B207" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H207" s="10" t="inlineStr">
@@ -4951,7 +4951,7 @@
       </c>
       <c r="B208" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H208" s="10" t="inlineStr">
@@ -4969,7 +4969,7 @@
       </c>
       <c r="B209" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H209" s="10" t="inlineStr">
@@ -4987,7 +4987,7 @@
       </c>
       <c r="B210" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H210" s="10" t="inlineStr">
@@ -5005,7 +5005,7 @@
       </c>
       <c r="B211" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H211" s="10" t="inlineStr">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="B212" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H212" s="10" t="inlineStr">
@@ -5041,7 +5041,7 @@
       </c>
       <c r="B213" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H213" s="10" t="inlineStr">
@@ -5059,7 +5059,7 @@
       </c>
       <c r="B214" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H214" s="10" t="inlineStr">
@@ -5077,7 +5077,7 @@
       </c>
       <c r="B215" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H215" s="10" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="B216" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H216" s="10" t="inlineStr">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="B217" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H217" s="10" t="inlineStr">
@@ -5131,7 +5131,7 @@
       </c>
       <c r="B218" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H218" s="10" t="inlineStr">
@@ -5149,7 +5149,7 @@
       </c>
       <c r="B219" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H219" s="10" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="B220" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H220" s="10" t="inlineStr">
@@ -5185,7 +5185,7 @@
       </c>
       <c r="B221" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H221" s="10" t="inlineStr">
@@ -5203,7 +5203,7 @@
       </c>
       <c r="B222" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H222" s="10" t="inlineStr">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="B223" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H223" s="10" t="inlineStr">
@@ -5239,7 +5239,7 @@
       </c>
       <c r="B224" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H224" s="10" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B225" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H225" s="10" t="inlineStr">
@@ -5275,7 +5275,7 @@
       </c>
       <c r="B226" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H226" s="10" t="inlineStr">
@@ -5293,7 +5293,7 @@
       </c>
       <c r="B227" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H227" s="10" t="inlineStr">
@@ -5311,7 +5311,7 @@
       </c>
       <c r="B228" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H228" s="10" t="inlineStr">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="B229" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H229" s="10" t="inlineStr">
@@ -5347,7 +5347,7 @@
       </c>
       <c r="B230" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H230" s="10" t="inlineStr">
@@ -5365,7 +5365,7 @@
       </c>
       <c r="B231" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H231" s="10" t="inlineStr">
@@ -5383,7 +5383,7 @@
       </c>
       <c r="B232" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H232" s="10" t="inlineStr">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="B233" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H233" s="10" t="inlineStr">
@@ -5419,7 +5419,7 @@
       </c>
       <c r="B234" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H234" s="10" t="inlineStr">
@@ -5437,7 +5437,7 @@
       </c>
       <c r="B235" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H235" s="10" t="inlineStr">
@@ -5455,7 +5455,7 @@
       </c>
       <c r="B236" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H236" s="10" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="B237" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H237" s="10" t="inlineStr">
@@ -5491,7 +5491,7 @@
       </c>
       <c r="B238" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H238" s="10" t="inlineStr">
@@ -5509,7 +5509,7 @@
       </c>
       <c r="B239" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H239" s="10" t="inlineStr">
@@ -5527,7 +5527,7 @@
       </c>
       <c r="B240" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H240" s="10" t="inlineStr">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="B241" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H241" s="10" t="inlineStr">
@@ -5563,7 +5563,7 @@
       </c>
       <c r="B242" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H242" s="10" t="inlineStr">
@@ -5581,7 +5581,7 @@
       </c>
       <c r="B243" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H243" s="10" t="inlineStr">
@@ -5599,7 +5599,7 @@
       </c>
       <c r="B244" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H244" s="10" t="inlineStr">
@@ -5617,7 +5617,7 @@
       </c>
       <c r="B245" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H245" s="10" t="inlineStr">
@@ -5635,7 +5635,7 @@
       </c>
       <c r="B246" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H246" s="10" t="inlineStr">
@@ -5653,7 +5653,7 @@
       </c>
       <c r="B247" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H247" s="10" t="inlineStr">
@@ -5671,7 +5671,7 @@
       </c>
       <c r="B248" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H248" s="10" t="inlineStr">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="B249" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H249" s="10" t="inlineStr">
@@ -5707,7 +5707,7 @@
       </c>
       <c r="B250" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H250" s="10" t="inlineStr">
@@ -5725,7 +5725,7 @@
       </c>
       <c r="B251" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H251" s="10" t="inlineStr">
@@ -5743,7 +5743,7 @@
       </c>
       <c r="B252" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H252" s="10" t="inlineStr">
@@ -5761,7 +5761,7 @@
       </c>
       <c r="B253" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H253" s="10" t="inlineStr">
@@ -5779,7 +5779,7 @@
       </c>
       <c r="B254" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H254" s="10" t="inlineStr">
@@ -5797,7 +5797,7 @@
       </c>
       <c r="B255" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H255" s="10" t="inlineStr">
@@ -5815,7 +5815,7 @@
       </c>
       <c r="B256" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H256" s="10" t="inlineStr">
@@ -5833,7 +5833,7 @@
       </c>
       <c r="B257" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H257" s="10" t="inlineStr">
@@ -5851,7 +5851,7 @@
       </c>
       <c r="B258" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H258" s="10" t="inlineStr">
@@ -5869,7 +5869,7 @@
       </c>
       <c r="B259" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H259" s="10" t="inlineStr">
@@ -5887,7 +5887,7 @@
       </c>
       <c r="B260" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H260" s="10" t="inlineStr">
@@ -5905,7 +5905,7 @@
       </c>
       <c r="B261" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H261" s="10" t="inlineStr">
@@ -5923,7 +5923,7 @@
       </c>
       <c r="B262" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H262" s="10" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="B263" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H263" s="10" t="inlineStr">
@@ -5959,7 +5959,7 @@
       </c>
       <c r="B264" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H264" s="10" t="inlineStr">
@@ -5977,7 +5977,7 @@
       </c>
       <c r="B265" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H265" s="10" t="inlineStr">
@@ -5995,7 +5995,7 @@
       </c>
       <c r="B266" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H266" s="10" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="B267" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H267" s="10" t="inlineStr">
@@ -6031,7 +6031,7 @@
       </c>
       <c r="B268" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H268" s="10" t="inlineStr">
@@ -6049,7 +6049,7 @@
       </c>
       <c r="B269" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H269" s="10" t="inlineStr">
@@ -6067,7 +6067,7 @@
       </c>
       <c r="B270" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H270" s="10" t="inlineStr">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="B271" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H271" s="10" t="inlineStr">
@@ -6103,7 +6103,7 @@
       </c>
       <c r="B272" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H272" s="10" t="inlineStr">
@@ -6121,7 +6121,7 @@
       </c>
       <c r="B273" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H273" s="10" t="inlineStr">
@@ -6139,7 +6139,7 @@
       </c>
       <c r="B274" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H274" s="10" t="inlineStr">
@@ -6157,7 +6157,7 @@
       </c>
       <c r="B275" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H275" s="10" t="inlineStr">
@@ -6175,7 +6175,7 @@
       </c>
       <c r="B276" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H276" s="10" t="inlineStr">
@@ -6193,7 +6193,7 @@
       </c>
       <c r="B277" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H277" s="10" t="inlineStr">
@@ -6211,7 +6211,7 @@
       </c>
       <c r="B278" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H278" s="10" t="inlineStr">
@@ -6229,7 +6229,7 @@
       </c>
       <c r="B279" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H279" s="10" t="inlineStr">
@@ -6247,7 +6247,7 @@
       </c>
       <c r="B280" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H280" s="10" t="inlineStr">
@@ -6265,7 +6265,7 @@
       </c>
       <c r="B281" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H281" s="10" t="inlineStr">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="B282" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H282" s="10" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="B283" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H283" s="10" t="inlineStr">
@@ -6319,7 +6319,7 @@
       </c>
       <c r="B284" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H284" s="10" t="inlineStr">
@@ -6337,7 +6337,7 @@
       </c>
       <c r="B285" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H285" s="10" t="inlineStr">
@@ -6355,7 +6355,7 @@
       </c>
       <c r="B286" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H286" s="10" t="inlineStr">
@@ -6373,7 +6373,7 @@
       </c>
       <c r="B287" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H287" s="10" t="inlineStr">
@@ -6391,7 +6391,7 @@
       </c>
       <c r="B288" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H288" s="10" t="inlineStr">
@@ -6409,7 +6409,7 @@
       </c>
       <c r="B289" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H289" s="10" t="inlineStr">
@@ -6427,7 +6427,7 @@
       </c>
       <c r="B290" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H290" s="10" t="inlineStr">
@@ -6445,7 +6445,7 @@
       </c>
       <c r="B291" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H291" s="10" t="inlineStr">
@@ -6463,7 +6463,7 @@
       </c>
       <c r="B292" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H292" s="10" t="inlineStr">
@@ -6481,7 +6481,7 @@
       </c>
       <c r="B293" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H293" s="10" t="inlineStr">
@@ -6499,7 +6499,7 @@
       </c>
       <c r="B294" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H294" s="10" t="inlineStr">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="B295" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H295" s="10" t="inlineStr">
@@ -6535,7 +6535,7 @@
       </c>
       <c r="B296" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H296" s="10" t="inlineStr">
@@ -6553,7 +6553,7 @@
       </c>
       <c r="B297" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H297" s="10" t="inlineStr">
@@ -6571,7 +6571,7 @@
       </c>
       <c r="B298" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H298" s="10" t="inlineStr">
@@ -6589,7 +6589,7 @@
       </c>
       <c r="B299" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H299" s="10" t="inlineStr">
@@ -6607,7 +6607,7 @@
       </c>
       <c r="B300" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H300" s="10" t="inlineStr">
@@ -6625,7 +6625,7 @@
       </c>
       <c r="B301" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H301" s="10" t="inlineStr">
@@ -6643,7 +6643,7 @@
       </c>
       <c r="B302" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H302" s="10" t="inlineStr">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="B303" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H303" s="10" t="inlineStr">
@@ -6679,7 +6679,7 @@
       </c>
       <c r="B304" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H304" s="10" t="inlineStr">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="B305" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H305" s="10" t="inlineStr">
@@ -6715,7 +6715,7 @@
       </c>
       <c r="B306" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H306" s="10" t="inlineStr">
@@ -6733,7 +6733,7 @@
       </c>
       <c r="B307" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H307" s="10" t="inlineStr">
@@ -6751,7 +6751,7 @@
       </c>
       <c r="B308" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H308" s="10" t="inlineStr">
@@ -6769,7 +6769,7 @@
       </c>
       <c r="B309" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H309" s="10" t="inlineStr">
@@ -6787,7 +6787,7 @@
       </c>
       <c r="B310" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H310" s="10" t="inlineStr">
@@ -6805,7 +6805,7 @@
       </c>
       <c r="B311" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H311" s="10" t="inlineStr">
@@ -6823,7 +6823,7 @@
       </c>
       <c r="B312" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H312" s="10" t="inlineStr">

</xml_diff>

<commit_message>
pause and exe time for exceution works
</commit_message>
<xml_diff>
--- a/RotoDNFStats.xlsx
+++ b/RotoDNFStats.xlsx
@@ -7687,7 +7687,7 @@
       </c>
       <c r="B360" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H360" s="10" t="inlineStr">
@@ -7705,7 +7705,7 @@
       </c>
       <c r="B361" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H361" s="10" t="inlineStr">
@@ -7723,7 +7723,7 @@
       </c>
       <c r="B362" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H362" s="10" t="inlineStr">
@@ -7741,7 +7741,7 @@
       </c>
       <c r="B363" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H363" s="10" t="inlineStr">
@@ -7759,7 +7759,7 @@
       </c>
       <c r="B364" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H364" s="10" t="inlineStr">
@@ -7777,7 +7777,7 @@
       </c>
       <c r="B365" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H365" s="10" t="inlineStr">
@@ -7795,7 +7795,7 @@
       </c>
       <c r="B366" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H366" s="10" t="inlineStr">
@@ -7813,7 +7813,7 @@
       </c>
       <c r="B367" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H367" s="10" t="inlineStr">
@@ -7831,7 +7831,7 @@
       </c>
       <c r="B368" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H368" s="10" t="inlineStr">
@@ -7849,7 +7849,7 @@
       </c>
       <c r="B369" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H369" s="10" t="inlineStr">
@@ -7867,7 +7867,7 @@
       </c>
       <c r="B370" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H370" s="10" t="inlineStr">
@@ -7885,7 +7885,7 @@
       </c>
       <c r="B371" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H371" s="10" t="inlineStr">
@@ -7903,7 +7903,7 @@
       </c>
       <c r="B372" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H372" s="10" t="inlineStr">
@@ -7921,7 +7921,7 @@
       </c>
       <c r="B373" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H373" s="10" t="inlineStr">
@@ -7939,7 +7939,7 @@
       </c>
       <c r="B374" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H374" s="10" t="inlineStr">
@@ -7957,7 +7957,7 @@
       </c>
       <c r="B375" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H375" s="10" t="inlineStr">
@@ -7975,7 +7975,7 @@
       </c>
       <c r="B376" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H376" s="10" t="inlineStr">
@@ -7993,7 +7993,7 @@
       </c>
       <c r="B377" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H377" s="10" t="inlineStr">
@@ -8011,7 +8011,7 @@
       </c>
       <c r="B378" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H378" s="10" t="inlineStr">
@@ -8029,7 +8029,7 @@
       </c>
       <c r="B379" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H379" s="10" t="inlineStr">
@@ -8047,7 +8047,7 @@
       </c>
       <c r="B380" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H380" s="10" t="inlineStr">
@@ -8065,7 +8065,7 @@
       </c>
       <c r="B381" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H381" s="10" t="inlineStr">
@@ -8083,7 +8083,7 @@
       </c>
       <c r="B382" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H382" s="10" t="inlineStr">
@@ -8101,7 +8101,7 @@
       </c>
       <c r="B383" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H383" s="10" t="inlineStr">
@@ -8119,7 +8119,7 @@
       </c>
       <c r="B384" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H384" s="10" t="inlineStr">
@@ -8137,7 +8137,7 @@
       </c>
       <c r="B385" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H385" s="10" t="inlineStr">
@@ -8155,7 +8155,7 @@
       </c>
       <c r="B386" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H386" s="10" t="inlineStr">
@@ -8173,7 +8173,7 @@
       </c>
       <c r="B387" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H387" s="10" t="inlineStr">
@@ -8191,7 +8191,7 @@
       </c>
       <c r="B388" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H388" s="10" t="inlineStr">
@@ -8209,7 +8209,7 @@
       </c>
       <c r="B389" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H389" s="10" t="inlineStr">
@@ -8227,7 +8227,7 @@
       </c>
       <c r="B390" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H390" s="10" t="inlineStr">
@@ -8245,7 +8245,7 @@
       </c>
       <c r="B391" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H391" s="10" t="inlineStr">
@@ -8263,7 +8263,7 @@
       </c>
       <c r="B392" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H392" s="10" t="inlineStr">
@@ -8281,7 +8281,7 @@
       </c>
       <c r="B393" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H393" s="10" t="inlineStr">
@@ -8299,7 +8299,7 @@
       </c>
       <c r="B394" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H394" s="10" t="inlineStr">
@@ -8317,7 +8317,7 @@
       </c>
       <c r="B395" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H395" s="10" t="inlineStr">
@@ -8335,7 +8335,7 @@
       </c>
       <c r="B396" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H396" s="10" t="inlineStr">
@@ -8353,7 +8353,7 @@
       </c>
       <c r="B397" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H397" s="10" t="inlineStr">
@@ -8371,7 +8371,7 @@
       </c>
       <c r="B398" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H398" s="10" t="inlineStr">
@@ -8389,7 +8389,7 @@
       </c>
       <c r="B399" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H399" s="10" t="inlineStr">
@@ -8407,7 +8407,7 @@
       </c>
       <c r="B400" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H400" s="10" t="inlineStr">
@@ -8425,7 +8425,7 @@
       </c>
       <c r="B401" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H401" s="10" t="inlineStr">
@@ -8443,7 +8443,7 @@
       </c>
       <c r="B402" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H402" s="10" t="inlineStr">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="B403" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H403" s="10" t="inlineStr">
@@ -8479,7 +8479,7 @@
       </c>
       <c r="B404" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H404" s="10" t="inlineStr">
@@ -8497,7 +8497,7 @@
       </c>
       <c r="B405" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H405" s="10" t="inlineStr">
@@ -8515,7 +8515,7 @@
       </c>
       <c r="B406" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H406" s="10" t="inlineStr">
@@ -8533,7 +8533,7 @@
       </c>
       <c r="B407" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H407" s="10" t="inlineStr">
@@ -8551,7 +8551,7 @@
       </c>
       <c r="B408" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H408" s="10" t="inlineStr">
@@ -8569,7 +8569,7 @@
       </c>
       <c r="B409" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H409" s="10" t="inlineStr">
@@ -8587,7 +8587,7 @@
       </c>
       <c r="B410" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H410" s="10" t="inlineStr">
@@ -8605,7 +8605,7 @@
       </c>
       <c r="B411" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H411" s="10" t="inlineStr">
@@ -8623,7 +8623,7 @@
       </c>
       <c r="B412" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H412" s="10" t="inlineStr">
@@ -8641,7 +8641,7 @@
       </c>
       <c r="B413" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H413" s="10" t="inlineStr">
@@ -8659,7 +8659,7 @@
       </c>
       <c r="B414" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H414" s="10" t="inlineStr">
@@ -8677,7 +8677,7 @@
       </c>
       <c r="B415" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H415" s="10" t="inlineStr">
@@ -8695,7 +8695,7 @@
       </c>
       <c r="B416" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H416" s="10" t="inlineStr">
@@ -8713,7 +8713,7 @@
       </c>
       <c r="B417" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H417" s="10" t="inlineStr">
@@ -8731,7 +8731,7 @@
       </c>
       <c r="B418" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H418" s="10" t="inlineStr">
@@ -8749,7 +8749,7 @@
       </c>
       <c r="B419" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H419" s="10" t="inlineStr">
@@ -8767,7 +8767,7 @@
       </c>
       <c r="B420" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H420" s="10" t="inlineStr">
@@ -8785,7 +8785,7 @@
       </c>
       <c r="B421" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H421" s="10" t="inlineStr">
@@ -8803,7 +8803,7 @@
       </c>
       <c r="B422" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H422" s="10" t="inlineStr">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="B423" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H423" s="10" t="inlineStr">
@@ -8839,7 +8839,7 @@
       </c>
       <c r="B424" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H424" s="10" t="inlineStr">
@@ -8857,7 +8857,7 @@
       </c>
       <c r="B425" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H425" s="10" t="inlineStr">
@@ -8875,7 +8875,7 @@
       </c>
       <c r="B426" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H426" s="10" t="inlineStr">
@@ -8893,7 +8893,7 @@
       </c>
       <c r="B427" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H427" s="10" t="inlineStr">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="B428" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H428" s="10" t="inlineStr">
@@ -8929,7 +8929,7 @@
       </c>
       <c r="B429" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H429" s="10" t="inlineStr">
@@ -8947,7 +8947,7 @@
       </c>
       <c r="B430" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H430" s="10" t="inlineStr">
@@ -8965,7 +8965,7 @@
       </c>
       <c r="B431" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H431" s="10" t="inlineStr">
@@ -8983,7 +8983,7 @@
       </c>
       <c r="B432" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H432" s="10" t="inlineStr">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="B433" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H433" s="10" t="inlineStr">
@@ -9019,7 +9019,7 @@
       </c>
       <c r="B434" s="1" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="H434" s="10" t="inlineStr">

</xml_diff>